<commit_message>
Final - Italy win
</commit_message>
<xml_diff>
--- a/competition/Euro 2020 Fixtures.xlsx
+++ b/competition/Euro 2020 Fixtures.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Footy\Euro 2020\competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B023911-3B5B-4DE6-B68A-E2B2F584F38E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E24809-99D3-4809-8E7A-4135BE262BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,8 @@
     <sheet name="Fixtures - Template" sheetId="27" state="hidden" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Goals!$A$1:$I$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Fixtures!$A$1:$L$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Goals!$A$1:$I$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1996" uniqueCount="323">
   <si>
     <t>Date</t>
   </si>
@@ -741,21 +742,9 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>M. Demeril</t>
-  </si>
-  <si>
-    <t>C. Immobile</t>
-  </si>
-  <si>
-    <t>L. Insigne</t>
-  </si>
-  <si>
     <t>Joel Pohjanpalo</t>
   </si>
   <si>
-    <t>SUI</t>
-  </si>
-  <si>
     <t>Breel Embolo</t>
   </si>
   <si>
@@ -801,9 +790,6 @@
     <t>Patrik Schick</t>
   </si>
   <si>
-    <t>CZH</t>
-  </si>
-  <si>
     <t>Wojciech Szczesny</t>
   </si>
   <si>
@@ -811,6 +797,225 @@
   </si>
   <si>
     <t>Milan Škriniar</t>
+  </si>
+  <si>
+    <t>Raphaël Guerreiro</t>
+  </si>
+  <si>
+    <t>Cristiano Ronaldo</t>
+  </si>
+  <si>
+    <t>Mats Hummels</t>
+  </si>
+  <si>
+    <t>Swizterland</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Aleksei Miranchuk</t>
+  </si>
+  <si>
+    <t>Aaron Ramsey</t>
+  </si>
+  <si>
+    <t>Gareth Bale</t>
+  </si>
+  <si>
+    <t>Manuel Locatelli</t>
+  </si>
+  <si>
+    <t>Ciro Immobile</t>
+  </si>
+  <si>
+    <t>Merih Demeril</t>
+  </si>
+  <si>
+    <t>Lorenzo Insigne</t>
+  </si>
+  <si>
+    <t>Ezgjan Alioski</t>
+  </si>
+  <si>
+    <t>Yussuf Polsen</t>
+  </si>
+  <si>
+    <t>Thorgan Hazard</t>
+  </si>
+  <si>
+    <t>Kevin DeBruyne</t>
+  </si>
+  <si>
+    <t>Memphis Depay</t>
+  </si>
+  <si>
+    <t>Emil Forsberg</t>
+  </si>
+  <si>
+    <t>Ivan Perisic</t>
+  </si>
+  <si>
+    <t>Attila Fiola</t>
+  </si>
+  <si>
+    <t>Antionne Greizmann</t>
+  </si>
+  <si>
+    <t>Ruben Diaz</t>
+  </si>
+  <si>
+    <t>Kai Havertz</t>
+  </si>
+  <si>
+    <t>Robin Gosens</t>
+  </si>
+  <si>
+    <t>Diogo Gota</t>
+  </si>
+  <si>
+    <t>Robert Lewandowski</t>
+  </si>
+  <si>
+    <t>Matteo Pessina</t>
+  </si>
+  <si>
+    <t>Haris Seferovic</t>
+  </si>
+  <si>
+    <t>Xherdan Shaqiri</t>
+  </si>
+  <si>
+    <t>İrfan Can Kahveci</t>
+  </si>
+  <si>
+    <t>Cristoff Baumgartner</t>
+  </si>
+  <si>
+    <t>Lukas Hradecky</t>
+  </si>
+  <si>
+    <t>Mikkel Damsgaard</t>
+  </si>
+  <si>
+    <t>Andreas Christensen</t>
+  </si>
+  <si>
+    <t>Artem Dzyuba</t>
+  </si>
+  <si>
+    <t>Joakim Maehle</t>
+  </si>
+  <si>
+    <t>Nikola Vlasic</t>
+  </si>
+  <si>
+    <t>Callum McGregor</t>
+  </si>
+  <si>
+    <t>Luka Modric</t>
+  </si>
+  <si>
+    <t>Viktor Claessen</t>
+  </si>
+  <si>
+    <t>Martin Dubravka</t>
+  </si>
+  <si>
+    <t>Aymeric Laporte</t>
+  </si>
+  <si>
+    <t>Pablo Sarabia</t>
+  </si>
+  <si>
+    <t>Ferran Torres</t>
+  </si>
+  <si>
+    <t>Juraj Kucka</t>
+  </si>
+  <si>
+    <t>Adam Szalai</t>
+  </si>
+  <si>
+    <t>Andras Schafer</t>
+  </si>
+  <si>
+    <t>Leon Goretzka</t>
+  </si>
+  <si>
+    <t>Karim Benzema</t>
+  </si>
+  <si>
+    <t>Kasper Dolberg</t>
+  </si>
+  <si>
+    <t>Martin Brathwaite</t>
+  </si>
+  <si>
+    <t>Federico Chiesa</t>
+  </si>
+  <si>
+    <t>Sasa Kalajdzic</t>
+  </si>
+  <si>
+    <t>Tomas Holes</t>
+  </si>
+  <si>
+    <t>Thorgen Hazard</t>
+  </si>
+  <si>
+    <t>Pedri</t>
+  </si>
+  <si>
+    <t>Cesar Azpilicueta</t>
+  </si>
+  <si>
+    <t>Alvaro Morata</t>
+  </si>
+  <si>
+    <t>Mikel Oyarzabal</t>
+  </si>
+  <si>
+    <t>Mislav Orsic</t>
+  </si>
+  <si>
+    <t>Mario Pasalic</t>
+  </si>
+  <si>
+    <t>Paul Poga</t>
+  </si>
+  <si>
+    <t>Mario Gavranovic</t>
+  </si>
+  <si>
+    <t>Harry Kane</t>
+  </si>
+  <si>
+    <t>Oleksandr Zinchenko</t>
+  </si>
+  <si>
+    <t>Denis Zakaria</t>
+  </si>
+  <si>
+    <t>Nicolo Barella</t>
+  </si>
+  <si>
+    <t>Thomas Delaney</t>
+  </si>
+  <si>
+    <t>Harry Maguire</t>
+  </si>
+  <si>
+    <t>Jordan Henderson</t>
+  </si>
+  <si>
+    <t>Simon Kjaer</t>
+  </si>
+  <si>
+    <t>Luke Shaw</t>
+  </si>
+  <si>
+    <t>Leonardo Bonnucci</t>
   </si>
 </sst>
 </file>
@@ -950,7 +1155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1205,6 +1410,10 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12210,7 +12419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E25"/>
     </sheetView>
   </sheetViews>
@@ -12818,8 +13027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -12834,7 +13043,7 @@
     <col min="9" max="9" width="15.140625" style="21" customWidth="1"/>
     <col min="10" max="10" width="11" style="7" customWidth="1"/>
     <col min="11" max="11" width="12" style="7" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" style="7" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="7" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
@@ -13294,11 +13503,15 @@
       <c r="I12" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
+      <c r="J12" s="35">
+        <v>0</v>
+      </c>
+      <c r="K12" s="35">
+        <v>3</v>
+      </c>
       <c r="L12" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -13329,11 +13542,15 @@
       <c r="I13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
+      <c r="J13" s="35">
+        <v>1</v>
+      </c>
+      <c r="K13" s="35">
+        <v>0</v>
+      </c>
       <c r="L13" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>H</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -13364,11 +13581,15 @@
       <c r="I14" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
+      <c r="J14" s="35">
+        <v>0</v>
+      </c>
+      <c r="K14" s="35">
+        <v>1</v>
+      </c>
       <c r="L14" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -13399,11 +13620,15 @@
       <c r="I15" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
+      <c r="J15" s="35">
+        <v>0</v>
+      </c>
+      <c r="K15" s="35">
+        <v>2</v>
+      </c>
       <c r="L15" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -13434,11 +13659,15 @@
       <c r="I16" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
+      <c r="J16" s="35">
+        <v>3</v>
+      </c>
+      <c r="K16" s="35">
+        <v>0</v>
+      </c>
       <c r="L16" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>H</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -13469,11 +13698,15 @@
       <c r="I17" s="39" t="s">
         <v>202</v>
       </c>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
+      <c r="J17" s="35">
+        <v>2</v>
+      </c>
+      <c r="K17" s="35">
+        <v>1</v>
+      </c>
       <c r="L17" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>H</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -13504,11 +13737,15 @@
       <c r="I18" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
+      <c r="J18" s="35">
+        <v>1</v>
+      </c>
+      <c r="K18" s="35">
+        <v>2</v>
+      </c>
       <c r="L18" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -13539,11 +13776,15 @@
       <c r="I19" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
+      <c r="J19" s="35">
+        <v>2</v>
+      </c>
+      <c r="K19" s="35">
+        <v>0</v>
+      </c>
       <c r="L19" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>H</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -13574,11 +13815,15 @@
       <c r="I20" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
+      <c r="J20" s="35">
+        <v>1</v>
+      </c>
+      <c r="K20" s="35">
+        <v>0</v>
+      </c>
       <c r="L20" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>H</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -13609,11 +13854,15 @@
       <c r="I21" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
+      <c r="J21" s="35">
+        <v>1</v>
+      </c>
+      <c r="K21" s="35">
+        <v>1</v>
+      </c>
       <c r="L21" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>D</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -13644,11 +13893,15 @@
       <c r="I22" s="36" t="s">
         <v>204</v>
       </c>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
+      <c r="J22" s="35">
+        <v>0</v>
+      </c>
+      <c r="K22" s="35">
+        <v>0</v>
+      </c>
       <c r="L22" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>D</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -13679,11 +13932,15 @@
       <c r="I23" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
+      <c r="J23" s="35">
+        <v>1</v>
+      </c>
+      <c r="K23" s="35">
+        <v>1</v>
+      </c>
       <c r="L23" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>D</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -13714,11 +13971,15 @@
       <c r="I24" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
+      <c r="J24" s="35">
+        <v>2</v>
+      </c>
+      <c r="K24" s="35">
+        <v>4</v>
+      </c>
       <c r="L24" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -13749,11 +14010,15 @@
       <c r="I25" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
+      <c r="J25" s="35">
+        <v>1</v>
+      </c>
+      <c r="K25" s="35">
+        <v>1</v>
+      </c>
       <c r="L25" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>D</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -13784,11 +14049,15 @@
       <c r="I26" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="J26" s="35"/>
-      <c r="K26" s="35"/>
+      <c r="J26" s="35">
+        <v>1</v>
+      </c>
+      <c r="K26" s="35">
+        <v>0</v>
+      </c>
       <c r="L26" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>H</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -13819,11 +14088,15 @@
       <c r="I27" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="J27" s="35"/>
-      <c r="K27" s="35"/>
+      <c r="J27" s="35">
+        <v>3</v>
+      </c>
+      <c r="K27" s="35">
+        <v>1</v>
+      </c>
       <c r="L27" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>H</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -13854,11 +14127,15 @@
       <c r="I28" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="J28" s="35"/>
-      <c r="K28" s="35"/>
+      <c r="J28" s="35">
+        <v>0</v>
+      </c>
+      <c r="K28" s="35">
+        <v>1</v>
+      </c>
       <c r="L28" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -13889,11 +14166,15 @@
       <c r="I29" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="J29" s="35"/>
-      <c r="K29" s="35"/>
+      <c r="J29" s="35">
+        <v>0</v>
+      </c>
+      <c r="K29" s="35">
+        <v>3</v>
+      </c>
       <c r="L29" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -13924,11 +14205,15 @@
       <c r="I30" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="J30" s="35"/>
-      <c r="K30" s="35"/>
+      <c r="J30" s="35">
+        <v>0</v>
+      </c>
+      <c r="K30" s="35">
+        <v>2</v>
+      </c>
       <c r="L30" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
@@ -13959,11 +14244,15 @@
       <c r="I31" s="39" t="s">
         <v>198</v>
       </c>
-      <c r="J31" s="35"/>
-      <c r="K31" s="35"/>
+      <c r="J31" s="35">
+        <v>1</v>
+      </c>
+      <c r="K31" s="35">
+        <v>4</v>
+      </c>
       <c r="L31" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -13994,11 +14283,15 @@
       <c r="I32" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
+      <c r="J32" s="35">
+        <v>0</v>
+      </c>
+      <c r="K32" s="35">
+        <v>1</v>
+      </c>
       <c r="L32" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -14029,11 +14322,15 @@
       <c r="I33" s="39" t="s">
         <v>204</v>
       </c>
-      <c r="J33" s="35"/>
-      <c r="K33" s="35"/>
+      <c r="J33" s="35">
+        <v>3</v>
+      </c>
+      <c r="K33" s="35">
+        <v>1</v>
+      </c>
       <c r="L33" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>NPY</v>
+        <v>H</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
@@ -14064,11 +14361,15 @@
       <c r="I34" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="J34" s="35"/>
-      <c r="K34" s="35"/>
+      <c r="J34" s="35">
+        <v>3</v>
+      </c>
+      <c r="K34" s="35">
+        <v>2</v>
+      </c>
       <c r="L34" s="30" t="str">
         <f t="shared" ref="L34:L52" si="1">IF(AND(ISBLANK(J34),ISBLANK(K34)),"NPY",IF(J34&gt;K34,"H",IF(J34=K34,"D",IF(J34&lt;K34,"A"))))</f>
-        <v>NPY</v>
+        <v>H</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
@@ -14099,11 +14400,15 @@
       <c r="I35" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="J35" s="35"/>
-      <c r="K35" s="35"/>
+      <c r="J35" s="35">
+        <v>0</v>
+      </c>
+      <c r="K35" s="35">
+        <v>5</v>
+      </c>
       <c r="L35" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
@@ -14134,11 +14439,15 @@
       <c r="I36" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="J36" s="35"/>
-      <c r="K36" s="35"/>
+      <c r="J36" s="35">
+        <v>2</v>
+      </c>
+      <c r="K36" s="35">
+        <v>2</v>
+      </c>
       <c r="L36" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>D</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
@@ -14169,11 +14478,15 @@
       <c r="I37" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="J37" s="35"/>
-      <c r="K37" s="35"/>
+      <c r="J37" s="35">
+        <v>2</v>
+      </c>
+      <c r="K37" s="35">
+        <v>2</v>
+      </c>
       <c r="L37" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>D</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
@@ -14196,19 +14509,23 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="G38" s="54" t="s">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="H38" s="55" t="s">
         <v>174</v>
       </c>
       <c r="I38" s="56" t="s">
-        <v>103</v>
-      </c>
-      <c r="J38" s="55"/>
-      <c r="K38" s="55"/>
+        <v>198</v>
+      </c>
+      <c r="J38" s="55">
+        <v>0</v>
+      </c>
+      <c r="K38" s="55">
+        <v>4</v>
+      </c>
       <c r="L38" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="39" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.2">
@@ -14231,19 +14548,23 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="G39" s="54" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="H39" s="55" t="s">
         <v>174</v>
       </c>
       <c r="I39" s="56" t="s">
-        <v>109</v>
-      </c>
-      <c r="J39" s="55"/>
-      <c r="K39" s="55"/>
+        <v>153</v>
+      </c>
+      <c r="J39" s="55">
+        <v>2</v>
+      </c>
+      <c r="K39" s="55">
+        <v>1</v>
+      </c>
       <c r="L39" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>H</v>
       </c>
     </row>
     <row r="40" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.2">
@@ -14266,19 +14587,23 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="G40" s="54" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="H40" s="55" t="s">
         <v>174</v>
       </c>
       <c r="I40" s="56" t="s">
-        <v>226</v>
-      </c>
-      <c r="J40" s="55"/>
-      <c r="K40" s="55"/>
+        <v>157</v>
+      </c>
+      <c r="J40" s="55">
+        <v>0</v>
+      </c>
+      <c r="K40" s="55">
+        <v>2</v>
+      </c>
       <c r="L40" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="41" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.2">
@@ -14301,19 +14626,23 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="G41" s="54" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="H41" s="55" t="s">
         <v>174</v>
       </c>
       <c r="I41" s="56" t="s">
-        <v>227</v>
-      </c>
-      <c r="J41" s="55"/>
-      <c r="K41" s="55"/>
+        <v>12</v>
+      </c>
+      <c r="J41" s="55">
+        <v>1</v>
+      </c>
+      <c r="K41" s="55">
+        <v>0</v>
+      </c>
       <c r="L41" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>H</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.2">
@@ -14336,19 +14665,23 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="G42" s="54" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="H42" s="55" t="s">
         <v>174</v>
       </c>
       <c r="I42" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="J42" s="55"/>
-      <c r="K42" s="55"/>
+        <v>6</v>
+      </c>
+      <c r="J42" s="55">
+        <v>3</v>
+      </c>
+      <c r="K42" s="55">
+        <v>5</v>
+      </c>
       <c r="L42" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="43" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.2">
@@ -14371,19 +14704,23 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="G43" s="54" t="s">
-        <v>114</v>
+        <v>11</v>
       </c>
       <c r="H43" s="55" t="s">
         <v>174</v>
       </c>
       <c r="I43" s="56" t="s">
-        <v>228</v>
-      </c>
-      <c r="J43" s="55"/>
-      <c r="K43" s="55"/>
+        <v>78</v>
+      </c>
+      <c r="J43" s="55">
+        <v>4</v>
+      </c>
+      <c r="K43" s="55">
+        <v>5</v>
+      </c>
       <c r="L43" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="44" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.2">
@@ -14406,19 +14743,23 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="G44" s="54" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="H44" s="55" t="s">
         <v>174</v>
       </c>
       <c r="I44" s="56" t="s">
-        <v>111</v>
-      </c>
-      <c r="J44" s="55"/>
-      <c r="K44" s="55"/>
+        <v>10</v>
+      </c>
+      <c r="J44" s="55">
+        <v>2</v>
+      </c>
+      <c r="K44" s="55">
+        <v>0</v>
+      </c>
       <c r="L44" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>H</v>
       </c>
     </row>
     <row r="45" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.2">
@@ -14441,19 +14782,23 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="G45" s="58" t="s">
-        <v>110</v>
+        <v>156</v>
       </c>
       <c r="H45" s="55" t="s">
         <v>174</v>
       </c>
       <c r="I45" s="59" t="s">
-        <v>229</v>
-      </c>
-      <c r="J45" s="55"/>
-      <c r="K45" s="55"/>
+        <v>159</v>
+      </c>
+      <c r="J45" s="55">
+        <v>1</v>
+      </c>
+      <c r="K45" s="55">
+        <v>2</v>
+      </c>
       <c r="L45" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="46" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.2">
@@ -14475,20 +14820,26 @@
       <c r="F46" s="44">
         <v>0.70833333333333337</v>
       </c>
-      <c r="G46" s="49" t="s">
-        <v>178</v>
+      <c r="G46" s="49" t="str">
+        <f>IF(AND(ISBLANK(J43),ISBLANK(K43)),"Winner 42",IF(J43&gt;K43,G43,I43))</f>
+        <v>Switzerland</v>
       </c>
       <c r="H46" s="46" t="s">
         <v>174</v>
       </c>
-      <c r="I46" s="47" t="s">
-        <v>179</v>
-      </c>
-      <c r="J46" s="46"/>
-      <c r="K46" s="46"/>
+      <c r="I46" s="47" t="str">
+        <f>IF(AND(ISBLANK(J42),ISBLANK(K42)),"Winner 41",IF(J42&gt;K42,G42,I42))</f>
+        <v>Spain</v>
+      </c>
+      <c r="J46" s="46">
+        <v>2</v>
+      </c>
+      <c r="K46" s="46">
+        <v>4</v>
+      </c>
       <c r="L46" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="47" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.2">
@@ -14510,20 +14861,26 @@
       <c r="F47" s="44">
         <v>0.83333333333333337</v>
       </c>
-      <c r="G47" s="45" t="s">
-        <v>181</v>
+      <c r="G47" s="45" t="str">
+        <f>IF(AND(ISBLANK(J41),ISBLANK(K41)),"Winner 40",IF(J41&gt;K41,G41,I41))</f>
+        <v>Belgium</v>
       </c>
       <c r="H47" s="46" t="s">
         <v>174</v>
       </c>
-      <c r="I47" s="47" t="s">
-        <v>177</v>
-      </c>
-      <c r="J47" s="46"/>
-      <c r="K47" s="46"/>
+      <c r="I47" s="47" t="str">
+        <f>IF(AND(ISBLANK(J39),ISBLANK(K39)),"Winner 38",IF(J39&gt;K39,G39,I39))</f>
+        <v>Italy</v>
+      </c>
+      <c r="J47" s="46">
+        <v>1</v>
+      </c>
+      <c r="K47" s="46">
+        <v>2</v>
+      </c>
       <c r="L47" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="48" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.2">
@@ -14545,20 +14902,26 @@
       <c r="F48" s="44">
         <v>0.70833333333333337</v>
       </c>
-      <c r="G48" s="45" t="s">
-        <v>176</v>
+      <c r="G48" s="45" t="str">
+        <f>IF(AND(ISBLANK(J40),ISBLANK(K40)),"Winner 39",IF(J40&gt;K40,G40,I40))</f>
+        <v>Czech Republic</v>
       </c>
       <c r="H48" s="46" t="s">
         <v>174</v>
       </c>
-      <c r="I48" s="47" t="s">
-        <v>175</v>
-      </c>
-      <c r="J48" s="46"/>
-      <c r="K48" s="46"/>
+      <c r="I48" s="47" t="str">
+        <f>IF(AND(ISBLANK(J38),ISBLANK(K38)),"Winner 37",IF(J38&gt;K38,G38,I38))</f>
+        <v>Denmark</v>
+      </c>
+      <c r="J48" s="46">
+        <v>1</v>
+      </c>
+      <c r="K48" s="46">
+        <v>2</v>
+      </c>
       <c r="L48" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="49" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.2">
@@ -14580,20 +14943,26 @@
       <c r="F49" s="44">
         <v>0.83333333333333337</v>
       </c>
-      <c r="G49" s="45" t="s">
-        <v>182</v>
+      <c r="G49" s="45" t="str">
+        <f>IF(AND(ISBLANK(J45),ISBLANK(K45)),"Winner 44",IF(J45&gt;K45,G45,I45))</f>
+        <v>Ukraine</v>
       </c>
       <c r="H49" s="46" t="s">
         <v>174</v>
       </c>
-      <c r="I49" s="47" t="s">
-        <v>180</v>
-      </c>
-      <c r="J49" s="46"/>
-      <c r="K49" s="46"/>
+      <c r="I49" s="47" t="str">
+        <f>IF(AND(ISBLANK(J44),ISBLANK(K44)),"Winner 43",IF(J44&gt;K44,G44,I44))</f>
+        <v>England</v>
+      </c>
+      <c r="J49" s="46">
+        <v>0</v>
+      </c>
+      <c r="K49" s="46">
+        <v>4</v>
+      </c>
       <c r="L49" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>A</v>
       </c>
     </row>
     <row r="50" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.2">
@@ -14615,20 +14984,26 @@
       <c r="F50" s="70">
         <v>0.83333333333333337</v>
       </c>
-      <c r="G50" s="71" t="s">
-        <v>184</v>
+      <c r="G50" s="71" t="str">
+        <f>IF(AND(ISBLANK(J47),ISBLANK(K47)),"Winner 46",IF(J47&gt;K47,G47,I47))</f>
+        <v>Italy</v>
       </c>
       <c r="H50" s="72" t="s">
         <v>174</v>
       </c>
-      <c r="I50" s="73" t="s">
-        <v>183</v>
-      </c>
-      <c r="J50" s="72"/>
-      <c r="K50" s="72"/>
+      <c r="I50" s="73" t="str">
+        <f>IF(AND(ISBLANK(J46),ISBLANK(K46)),"Winner 45",IF(J46&gt;K46,G46,I46))</f>
+        <v>Spain</v>
+      </c>
+      <c r="J50" s="72">
+        <v>4</v>
+      </c>
+      <c r="K50" s="72">
+        <v>2</v>
+      </c>
       <c r="L50" s="67" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>H</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
@@ -14650,20 +15025,26 @@
       <c r="F51" s="70">
         <v>0.83333333333333337</v>
       </c>
-      <c r="G51" s="71" t="s">
-        <v>186</v>
+      <c r="G51" s="71" t="str">
+        <f>IF(AND(ISBLANK(J49),ISBLANK(K49)),"Winner 48",IF(J49&gt;K49,G49,I49))</f>
+        <v>England</v>
       </c>
       <c r="H51" s="72" t="s">
         <v>174</v>
       </c>
-      <c r="I51" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="J51" s="72"/>
-      <c r="K51" s="72"/>
+      <c r="I51" s="73" t="str">
+        <f>IF(AND(ISBLANK(J48),ISBLANK(K48)),"Winner 47",IF(J48&gt;K48,G48,I48))</f>
+        <v>Denmark</v>
+      </c>
+      <c r="J51" s="72">
+        <v>2</v>
+      </c>
+      <c r="K51" s="72">
+        <v>1</v>
+      </c>
       <c r="L51" s="67" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>H</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -14685,23 +15066,30 @@
       <c r="F52" s="63">
         <v>0.83333333333333337</v>
       </c>
-      <c r="G52" s="64" t="s">
-        <v>118</v>
+      <c r="G52" s="64" t="str">
+        <f>IF(AND(ISBLANK(J50),ISBLANK(K50)),"Winner 49",IF(J50&gt;K50,G50,I50))</f>
+        <v>Italy</v>
       </c>
       <c r="H52" s="65" t="s">
         <v>174</v>
       </c>
-      <c r="I52" s="66" t="s">
-        <v>119</v>
-      </c>
-      <c r="J52" s="65"/>
-      <c r="K52" s="65"/>
+      <c r="I52" s="66" t="str">
+        <f>IF(AND(ISBLANK(J51),ISBLANK(K51)),"Winner 50",IF(J51&gt;K51,G51,I51))</f>
+        <v>England</v>
+      </c>
+      <c r="J52" s="65">
+        <v>4</v>
+      </c>
+      <c r="K52" s="65">
+        <v>3</v>
+      </c>
       <c r="L52" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>NPY</v>
+        <v>H</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L52" xr:uid="{00000000-0001-0000-0600-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L52">
     <sortCondition ref="A2:A52"/>
   </sortState>
@@ -14712,21 +15100,22 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="75"/>
     <col min="2" max="2" width="22.85546875" style="84" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="84" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="84" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" style="75" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="74" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="74" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="74" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="75" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="75" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="75" customWidth="1"/>
     <col min="8" max="8" width="11" style="75" customWidth="1"/>
     <col min="9" max="9" width="10" style="75" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="74"/>
@@ -14740,18 +15129,18 @@
         <v>52</v>
       </c>
       <c r="C1" s="84" t="s">
-        <v>143</v>
+        <v>254</v>
       </c>
       <c r="D1" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="E1" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="74" t="s">
+      <c r="F1" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="75" t="s">
         <v>56</v>
       </c>
       <c r="H1" s="75" t="s">
@@ -14765,11 +15154,11 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="85" t="s">
-        <v>231</v>
+      <c r="B2" s="91" t="s">
+        <v>260</v>
       </c>
       <c r="C2" s="86" t="s">
-        <v>168</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6">
@@ -14785,11 +15174,11 @@
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="85" t="s">
-        <v>232</v>
+      <c r="B3" s="91" t="s">
+        <v>259</v>
       </c>
       <c r="C3" s="86" t="s">
-        <v>163</v>
+        <v>8</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6">
@@ -14802,11 +15191,11 @@
       <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="85" t="s">
-        <v>233</v>
+      <c r="B4" s="91" t="s">
+        <v>261</v>
       </c>
       <c r="C4" s="86" t="s">
-        <v>163</v>
+        <v>8</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6">
@@ -14820,10 +15209,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="85" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C5" s="86" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6">
@@ -14837,10 +15226,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="85" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C6" s="86" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6">
@@ -14854,10 +15243,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="88" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C7" s="86" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6">
@@ -14869,10 +15258,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="85" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C8" s="86" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D8" s="6">
         <v>10</v>
@@ -14884,10 +15273,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="85" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C9" s="86" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D9" s="6">
         <v>34</v>
@@ -14899,10 +15288,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="85" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C10" s="86" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6">
@@ -14914,10 +15303,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="85" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C11" s="86" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6">
@@ -14929,10 +15318,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="85" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C12" s="86" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
       <c r="D12" s="6">
         <v>18</v>
@@ -14944,10 +15333,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="91" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C13" s="90" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D13" s="6">
         <v>28</v>
@@ -14959,10 +15348,10 @@
         <v>6</v>
       </c>
       <c r="B14" s="88" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C14" s="86" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6">
@@ -14974,10 +15363,10 @@
         <v>6</v>
       </c>
       <c r="B15" s="89" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C15" s="90" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6">
@@ -14989,335 +15378,2245 @@
         <v>7</v>
       </c>
       <c r="B16" s="93" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C16" s="86" t="s">
-        <v>200</v>
+        <v>70</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="40">
         <v>7</v>
       </c>
       <c r="B17" s="92" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C17" s="86" t="s">
-        <v>200</v>
+        <v>70</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="40">
         <v>7</v>
       </c>
       <c r="B18" s="91" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C18" s="86" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="40">
         <v>7</v>
       </c>
       <c r="B19" s="92" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C19" s="86" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="40">
         <v>7</v>
       </c>
       <c r="B20" s="91" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C20" s="86" t="s">
-        <v>200</v>
+        <v>70</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="40">
         <v>8</v>
       </c>
       <c r="B21" s="85" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C21" s="90" t="s">
-        <v>251</v>
+        <v>157</v>
       </c>
       <c r="D21" s="6">
         <v>42</v>
       </c>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="40">
         <v>8</v>
       </c>
       <c r="B22" s="85" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C22" s="90" t="s">
-        <v>251</v>
+        <v>157</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="40">
         <v>9</v>
       </c>
       <c r="B23" s="85" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C23" s="90" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="D23" s="6">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I23" s="75" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="40">
         <v>9</v>
       </c>
       <c r="B24" s="85" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C24" s="90" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D24" s="6">
         <v>46</v>
       </c>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="40">
         <v>9</v>
       </c>
       <c r="B25" s="85" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C25" s="90" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="40">
+        <v>11</v>
+      </c>
+      <c r="B26" s="91" t="s">
+        <v>250</v>
+      </c>
+      <c r="C26" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="40">
+        <v>11</v>
+      </c>
+      <c r="B27" s="91" t="s">
+        <v>251</v>
+      </c>
+      <c r="C27" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6">
+        <v>42</v>
+      </c>
+      <c r="H27" s="75" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="40">
+        <v>11</v>
+      </c>
+      <c r="B28" s="91" t="s">
+        <v>251</v>
+      </c>
+      <c r="C28" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="40">
+        <v>12</v>
+      </c>
+      <c r="B29" s="91" t="s">
+        <v>252</v>
+      </c>
+      <c r="C29" s="90" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="6">
+        <v>20</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="I29" s="75" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="40">
+        <v>13</v>
+      </c>
+      <c r="B30" s="91" t="s">
+        <v>255</v>
+      </c>
+      <c r="C30" s="90" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="6">
+        <v>47</v>
+      </c>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="40">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="40"/>
-      <c r="B26" s="85"/>
-      <c r="C26" s="86"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="40"/>
-      <c r="B27" s="85"/>
-      <c r="C27" s="86"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="40"/>
-      <c r="B28" s="85"/>
-      <c r="C28" s="86"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="40"/>
-      <c r="B29" s="85"/>
-      <c r="C29" s="86"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="40"/>
-      <c r="B30" s="85"/>
-      <c r="C30" s="86"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="40"/>
-      <c r="B31" s="85"/>
-      <c r="C31" s="86"/>
-      <c r="D31" s="6"/>
+      <c r="B31" s="85" t="s">
+        <v>256</v>
+      </c>
+      <c r="C31" s="86" t="s">
+        <v>155</v>
+      </c>
+      <c r="D31" s="6">
+        <v>42</v>
+      </c>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="40"/>
-      <c r="B32" s="85"/>
-      <c r="C32" s="86"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="40">
+        <v>14</v>
+      </c>
+      <c r="B32" s="85" t="s">
+        <v>257</v>
+      </c>
+      <c r="C32" s="86" t="s">
+        <v>155</v>
+      </c>
       <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="40"/>
-      <c r="B33" s="85"/>
-      <c r="C33" s="86"/>
-      <c r="D33" s="6"/>
+      <c r="E32" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="40">
+        <v>15</v>
+      </c>
+      <c r="B33" s="91" t="s">
+        <v>258</v>
+      </c>
+      <c r="C33" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="6">
+        <v>26</v>
+      </c>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="40"/>
-      <c r="B34" s="85"/>
-      <c r="C34" s="86"/>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="40">
+        <v>15</v>
+      </c>
+      <c r="B34" s="91" t="s">
+        <v>258</v>
+      </c>
+      <c r="C34" s="86" t="s">
+        <v>8</v>
+      </c>
       <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="40"/>
-      <c r="B35" s="85"/>
-      <c r="C35" s="86"/>
+      <c r="E34" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="40">
+        <v>15</v>
+      </c>
+      <c r="B35" s="91" t="s">
+        <v>259</v>
+      </c>
+      <c r="C35" s="86" t="s">
+        <v>8</v>
+      </c>
       <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="40"/>
-      <c r="B36" s="85"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="40"/>
-      <c r="B37" s="85"/>
-      <c r="C37" s="86"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="85"/>
-      <c r="C38" s="86"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="85"/>
-      <c r="C39" s="86"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="85"/>
-      <c r="C40" s="86"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="85"/>
-      <c r="C41" s="86"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="85"/>
-      <c r="C42" s="86"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B43" s="85"/>
-      <c r="C43" s="86"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B44" s="85"/>
-      <c r="C44" s="86"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B45" s="85"/>
-      <c r="C45" s="86"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B46" s="85"/>
-      <c r="C46" s="86"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B47" s="85"/>
-      <c r="C47" s="86"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B48" s="85"/>
-      <c r="C48" s="86"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B49" s="85"/>
-      <c r="C49" s="86"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B50" s="85"/>
-      <c r="C50" s="86"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B51" s="85"/>
-      <c r="C51" s="86"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B52" s="85"/>
-      <c r="C52" s="86"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B53" s="85"/>
-      <c r="C53" s="86"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
+      <c r="E35" s="6">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="94">
+        <v>16</v>
+      </c>
+      <c r="B36" s="93" t="s">
+        <v>243</v>
+      </c>
+      <c r="C36" s="93" t="s">
+        <v>159</v>
+      </c>
+      <c r="D36" s="94">
+        <v>29</v>
+      </c>
+      <c r="E36" s="94"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="94">
+        <v>16</v>
+      </c>
+      <c r="B37" s="93" t="s">
+        <v>244</v>
+      </c>
+      <c r="C37" s="93" t="s">
+        <v>159</v>
+      </c>
+      <c r="D37" s="94">
+        <v>34</v>
+      </c>
+      <c r="E37" s="94"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="94">
+        <v>16</v>
+      </c>
+      <c r="B38" s="93" t="s">
+        <v>262</v>
+      </c>
+      <c r="C38" s="93" t="s">
+        <v>202</v>
+      </c>
+      <c r="D38" s="94"/>
+      <c r="E38" s="94">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="75">
+        <v>17</v>
+      </c>
+      <c r="B39" s="93" t="s">
+        <v>263</v>
+      </c>
+      <c r="C39" s="93" t="s">
+        <v>198</v>
+      </c>
+      <c r="D39" s="94">
+        <v>2</v>
+      </c>
+      <c r="E39" s="94"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="75">
+        <v>17</v>
+      </c>
+      <c r="B40" s="93" t="s">
+        <v>264</v>
+      </c>
+      <c r="C40" s="93" t="s">
+        <v>90</v>
+      </c>
+      <c r="D40" s="94"/>
+      <c r="E40" s="94">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="75">
+        <v>17</v>
+      </c>
+      <c r="B41" s="93" t="s">
+        <v>265</v>
+      </c>
+      <c r="C41" s="93" t="s">
+        <v>90</v>
+      </c>
+      <c r="D41" s="94"/>
+      <c r="E41" s="94">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="94">
+        <v>18</v>
+      </c>
+      <c r="B42" s="93" t="s">
+        <v>266</v>
+      </c>
+      <c r="C42" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="94">
+        <v>11</v>
+      </c>
+      <c r="E42" s="94"/>
+      <c r="F42" s="94"/>
+      <c r="G42" s="94"/>
+      <c r="H42" s="94" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="94">
+        <v>18</v>
+      </c>
+      <c r="B43" s="93" t="s">
+        <v>245</v>
+      </c>
+      <c r="C43" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="94"/>
+      <c r="E43" s="94">
+        <v>22</v>
+      </c>
+      <c r="F43" s="94"/>
+      <c r="G43" s="94"/>
+      <c r="H43" s="94"/>
+    </row>
+    <row r="44" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A44" s="94">
+        <v>19</v>
+      </c>
+      <c r="B44" s="93" t="s">
+        <v>267</v>
+      </c>
+      <c r="C44" s="93" t="s">
+        <v>156</v>
+      </c>
+      <c r="D44" s="94"/>
+      <c r="E44" s="94">
+        <v>32</v>
+      </c>
+      <c r="F44" s="94"/>
+      <c r="G44" s="94"/>
+      <c r="H44" s="94" t="s">
+        <v>230</v>
+      </c>
+      <c r="I44" s="94"/>
+    </row>
+    <row r="45" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A45" s="94">
+        <v>20</v>
+      </c>
+      <c r="B45" s="93" t="s">
+        <v>268</v>
+      </c>
+      <c r="C45" s="93" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="94">
+        <v>47</v>
+      </c>
+      <c r="E45" s="94"/>
+      <c r="F45" s="94"/>
+      <c r="G45" s="94"/>
+      <c r="H45" s="94"/>
+      <c r="I45" s="94"/>
+    </row>
+    <row r="46" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A46" s="94">
+        <v>20</v>
+      </c>
+      <c r="B46" s="93" t="s">
+        <v>246</v>
+      </c>
+      <c r="C46" s="93" t="s">
+        <v>157</v>
+      </c>
+      <c r="D46" s="94">
+        <v>37</v>
+      </c>
+      <c r="E46" s="94"/>
+      <c r="F46" s="94"/>
+      <c r="G46" s="94"/>
+      <c r="H46" s="94" t="s">
+        <v>230</v>
+      </c>
+      <c r="I46" s="94"/>
+    </row>
+    <row r="47" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A47" s="94">
+        <v>22</v>
+      </c>
+      <c r="B47" s="93" t="s">
+        <v>269</v>
+      </c>
+      <c r="C47" s="93" t="s">
+        <v>161</v>
+      </c>
+      <c r="D47" s="94">
+        <v>47</v>
+      </c>
+      <c r="E47" s="94"/>
+      <c r="F47" s="94"/>
+      <c r="G47" s="94"/>
+      <c r="H47" s="94"/>
+      <c r="I47" s="94"/>
+    </row>
+    <row r="48" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A48" s="94">
+        <v>22</v>
+      </c>
+      <c r="B48" s="93" t="s">
+        <v>270</v>
+      </c>
+      <c r="C48" s="93" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="94"/>
+      <c r="E48" s="94">
+        <v>21</v>
+      </c>
+      <c r="F48" s="94"/>
+      <c r="G48" s="94"/>
+      <c r="H48" s="94"/>
+      <c r="I48" s="94"/>
+    </row>
+    <row r="49" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A49" s="94">
+        <v>23</v>
+      </c>
+      <c r="B49" s="93" t="s">
+        <v>251</v>
+      </c>
+      <c r="C49" s="93" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="94">
+        <v>15</v>
+      </c>
+      <c r="E49" s="94"/>
+      <c r="F49" s="94"/>
+      <c r="G49" s="94"/>
+      <c r="H49" s="94"/>
+      <c r="I49" s="94"/>
+    </row>
+    <row r="50" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A50" s="94">
+        <v>23</v>
+      </c>
+      <c r="B50" s="93" t="s">
+        <v>271</v>
+      </c>
+      <c r="C50" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="94">
+        <v>35</v>
+      </c>
+      <c r="E50" s="94"/>
+      <c r="F50" s="94"/>
+      <c r="G50" s="94"/>
+      <c r="I50" s="94" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A51" s="94">
+        <v>23</v>
+      </c>
+      <c r="B51" s="93" t="s">
+        <v>250</v>
+      </c>
+      <c r="C51" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="94">
+        <v>39</v>
+      </c>
+      <c r="E51" s="94"/>
+      <c r="F51" s="94"/>
+      <c r="G51" s="94"/>
+      <c r="I51" s="94" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A52" s="94">
+        <v>23</v>
+      </c>
+      <c r="B52" s="93" t="s">
+        <v>272</v>
+      </c>
+      <c r="C52" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" s="94"/>
+      <c r="E52" s="94">
+        <v>6</v>
+      </c>
+      <c r="F52" s="94"/>
+      <c r="G52" s="94"/>
+      <c r="H52" s="94"/>
+      <c r="I52" s="94"/>
+    </row>
+    <row r="53" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A53" s="94">
+        <v>23</v>
+      </c>
+      <c r="B53" s="93" t="s">
+        <v>273</v>
+      </c>
+      <c r="C53" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" s="94"/>
+      <c r="E53" s="94">
+        <v>15</v>
+      </c>
+      <c r="F53" s="94"/>
+      <c r="G53" s="94"/>
+      <c r="H53" s="94"/>
+      <c r="I53" s="94"/>
+    </row>
+    <row r="54" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A54" s="94">
+        <v>23</v>
+      </c>
+      <c r="B54" s="93" t="s">
+        <v>274</v>
+      </c>
+      <c r="C54" s="93" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" s="94"/>
+      <c r="E54" s="94">
+        <v>22</v>
+      </c>
+      <c r="F54" s="94"/>
+      <c r="G54" s="94"/>
+      <c r="H54" s="94"/>
+      <c r="I54" s="94"/>
+    </row>
+    <row r="55" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A55" s="94">
+        <v>24</v>
+      </c>
+      <c r="B55" s="93" t="s">
+        <v>307</v>
+      </c>
+      <c r="C55" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="94">
+        <v>25</v>
+      </c>
+      <c r="E55" s="94"/>
+      <c r="F55" s="94"/>
+      <c r="G55" s="94"/>
+      <c r="H55" s="94"/>
+      <c r="I55" s="94"/>
+    </row>
+    <row r="56" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A56" s="94">
+        <v>24</v>
+      </c>
+      <c r="B56" s="93" t="s">
+        <v>275</v>
+      </c>
+      <c r="C56" s="93" t="s">
+        <v>154</v>
+      </c>
+      <c r="D56" s="94"/>
+      <c r="E56" s="94">
+        <v>9</v>
+      </c>
+      <c r="F56" s="94"/>
+      <c r="G56" s="94"/>
+      <c r="H56" s="94"/>
+      <c r="I56" s="94"/>
+    </row>
+    <row r="57" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A57" s="94">
+        <v>25</v>
+      </c>
+      <c r="B57" s="93" t="s">
+        <v>276</v>
+      </c>
+      <c r="C57" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="94">
+        <v>39</v>
+      </c>
+      <c r="E57" s="94"/>
+      <c r="F57" s="94"/>
+      <c r="G57" s="94"/>
+      <c r="H57" s="94"/>
+      <c r="I57" s="94"/>
+    </row>
+    <row r="58" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A58" s="94">
+        <v>26</v>
+      </c>
+      <c r="B58" s="93" t="s">
+        <v>277</v>
+      </c>
+      <c r="C58" s="93" t="s">
+        <v>78</v>
+      </c>
+      <c r="D58" s="94">
+        <v>6</v>
+      </c>
+      <c r="E58" s="94"/>
+      <c r="F58" s="94"/>
+      <c r="G58" s="94"/>
+      <c r="H58" s="94"/>
+      <c r="I58" s="94"/>
+    </row>
+    <row r="59" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A59" s="94">
+        <v>26</v>
+      </c>
+      <c r="B59" s="93" t="s">
+        <v>278</v>
+      </c>
+      <c r="C59" s="93" t="s">
+        <v>78</v>
+      </c>
+      <c r="D59" s="94">
+        <v>26</v>
+      </c>
+      <c r="E59" s="94"/>
+      <c r="F59" s="94"/>
+      <c r="G59" s="94"/>
+      <c r="H59" s="94"/>
+      <c r="I59" s="94"/>
+    </row>
+    <row r="60" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A60" s="94">
+        <v>26</v>
+      </c>
+      <c r="B60" s="93" t="s">
+        <v>279</v>
+      </c>
+      <c r="C60" s="93" t="s">
+        <v>158</v>
+      </c>
+      <c r="D60" s="94"/>
+      <c r="E60" s="94">
+        <v>17</v>
+      </c>
+      <c r="F60" s="94"/>
+      <c r="G60" s="94"/>
+      <c r="H60" s="94"/>
+      <c r="I60" s="94"/>
+    </row>
+    <row r="61" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A61" s="94">
+        <v>26</v>
+      </c>
+      <c r="B61" s="93" t="s">
+        <v>278</v>
+      </c>
+      <c r="C61" s="93" t="s">
+        <v>78</v>
+      </c>
+      <c r="D61" s="94"/>
+      <c r="E61" s="94">
+        <v>22</v>
+      </c>
+      <c r="F61" s="94"/>
+      <c r="G61" s="94"/>
+      <c r="H61" s="94"/>
+      <c r="I61" s="94"/>
+    </row>
+    <row r="62" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A62" s="94">
+        <v>27</v>
+      </c>
+      <c r="B62" s="93" t="s">
+        <v>280</v>
+      </c>
+      <c r="C62" s="93" t="s">
+        <v>153</v>
+      </c>
+      <c r="D62" s="94">
+        <v>21</v>
+      </c>
+      <c r="E62" s="94"/>
+      <c r="F62" s="94"/>
+      <c r="G62" s="94"/>
+      <c r="H62" s="94"/>
+      <c r="I62" s="94"/>
+    </row>
+    <row r="63" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A63" s="94">
+        <v>28</v>
+      </c>
+      <c r="B63" s="93" t="s">
+        <v>266</v>
+      </c>
+      <c r="C63" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D63" s="94">
+        <v>24</v>
+      </c>
+      <c r="E63" s="94"/>
+      <c r="F63" s="94"/>
+      <c r="G63" s="94"/>
+      <c r="H63" s="94"/>
+      <c r="I63" s="94"/>
+    </row>
+    <row r="64" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A64" s="94">
+        <v>28</v>
+      </c>
+      <c r="B64" s="93" t="s">
+        <v>241</v>
+      </c>
+      <c r="C64" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D64" s="94"/>
+      <c r="E64" s="94">
+        <v>6</v>
+      </c>
+      <c r="F64" s="94"/>
+      <c r="G64" s="94"/>
+      <c r="H64" s="94"/>
+      <c r="I64" s="94"/>
+    </row>
+    <row r="65" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A65" s="94">
+        <v>28</v>
+      </c>
+      <c r="B65" s="93" t="s">
+        <v>241</v>
+      </c>
+      <c r="C65" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D65" s="94"/>
+      <c r="E65" s="94">
+        <v>13</v>
+      </c>
+      <c r="F65" s="94"/>
+      <c r="G65" s="94"/>
+      <c r="H65" s="94"/>
+      <c r="I65" s="94"/>
+    </row>
+    <row r="66" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A66" s="94">
+        <v>29</v>
+      </c>
+      <c r="B66" s="93" t="s">
+        <v>281</v>
+      </c>
+      <c r="C66" s="93" t="s">
+        <v>90</v>
+      </c>
+      <c r="D66" s="94"/>
+      <c r="E66" s="94">
+        <v>29</v>
+      </c>
+      <c r="F66" s="94"/>
+      <c r="G66" s="94"/>
+      <c r="H66" s="94"/>
+      <c r="I66" s="94" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A67" s="94">
+        <v>29</v>
+      </c>
+      <c r="B67" s="93" t="s">
+        <v>234</v>
+      </c>
+      <c r="C67" s="93" t="s">
+        <v>90</v>
+      </c>
+      <c r="D67" s="94"/>
+      <c r="E67" s="94">
+        <v>41</v>
+      </c>
+      <c r="F67" s="94"/>
+      <c r="G67" s="94"/>
+      <c r="H67" s="94"/>
+      <c r="I67" s="94"/>
+    </row>
+    <row r="68" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A68" s="94">
+        <v>30</v>
+      </c>
+      <c r="B68" s="93" t="s">
+        <v>282</v>
+      </c>
+      <c r="C68" s="93" t="s">
+        <v>198</v>
+      </c>
+      <c r="D68" s="94">
+        <v>38</v>
+      </c>
+      <c r="E68" s="94"/>
+      <c r="F68" s="94"/>
+      <c r="G68" s="94"/>
+      <c r="H68" s="94"/>
+      <c r="I68" s="94"/>
+    </row>
+    <row r="69" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A69" s="94">
+        <v>30</v>
+      </c>
+      <c r="B69" s="93" t="s">
+        <v>263</v>
+      </c>
+      <c r="C69" s="93" t="s">
+        <v>198</v>
+      </c>
+      <c r="D69" s="94"/>
+      <c r="E69" s="94">
+        <v>14</v>
+      </c>
+      <c r="F69" s="94"/>
+      <c r="G69" s="94"/>
+      <c r="H69" s="94"/>
+      <c r="I69" s="94"/>
+    </row>
+    <row r="70" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A70" s="94">
+        <v>30</v>
+      </c>
+      <c r="B70" s="95" t="s">
+        <v>284</v>
+      </c>
+      <c r="C70" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="94"/>
+      <c r="E70" s="94">
+        <v>25</v>
+      </c>
+      <c r="F70" s="94"/>
+      <c r="G70" s="94"/>
+      <c r="H70" s="94" t="s">
+        <v>230</v>
+      </c>
+      <c r="I70" s="94"/>
+    </row>
+    <row r="71" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A71" s="94">
+        <v>30</v>
+      </c>
+      <c r="B71" s="93" t="s">
+        <v>283</v>
+      </c>
+      <c r="C71" s="93" t="s">
+        <v>198</v>
+      </c>
+      <c r="D71" s="94"/>
+      <c r="E71" s="94">
+        <v>34</v>
+      </c>
+      <c r="F71" s="94"/>
+      <c r="G71" s="94"/>
+      <c r="H71" s="94"/>
+      <c r="I71" s="94"/>
+    </row>
+    <row r="72" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A72" s="94">
+        <v>30</v>
+      </c>
+      <c r="B72" s="93" t="s">
+        <v>285</v>
+      </c>
+      <c r="C72" s="93" t="s">
+        <v>198</v>
+      </c>
+      <c r="D72" s="94"/>
+      <c r="E72" s="94">
+        <v>37</v>
+      </c>
+      <c r="F72" s="94"/>
+      <c r="G72" s="94"/>
+      <c r="H72" s="94"/>
+      <c r="I72" s="94"/>
+    </row>
+    <row r="73" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A73" s="94">
+        <v>31</v>
+      </c>
+      <c r="B73" s="93" t="s">
+        <v>236</v>
+      </c>
+      <c r="C73" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" s="94">
+        <v>12</v>
+      </c>
+      <c r="E73" s="94"/>
+      <c r="F73" s="94"/>
+      <c r="G73" s="94"/>
+      <c r="H73" s="94"/>
+      <c r="I73" s="94"/>
+    </row>
+    <row r="74" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A74" s="94">
+        <v>32</v>
+      </c>
+      <c r="B74" s="93" t="s">
+        <v>286</v>
+      </c>
+      <c r="C74" s="93" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="94">
+        <v>17</v>
+      </c>
+      <c r="E74" s="94"/>
+      <c r="F74" s="94"/>
+      <c r="G74" s="94"/>
+      <c r="H74" s="94"/>
+      <c r="I74" s="94"/>
+    </row>
+    <row r="75" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A75" s="94">
+        <v>32</v>
+      </c>
+      <c r="B75" s="93" t="s">
+        <v>287</v>
+      </c>
+      <c r="C75" s="93" t="s">
+        <v>204</v>
+      </c>
+      <c r="D75" s="94">
+        <v>42</v>
+      </c>
+      <c r="E75" s="94"/>
+      <c r="F75" s="94"/>
+      <c r="G75" s="94"/>
+      <c r="H75" s="94"/>
+      <c r="I75" s="94"/>
+    </row>
+    <row r="76" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A76" s="94">
+        <v>32</v>
+      </c>
+      <c r="B76" s="93" t="s">
+        <v>288</v>
+      </c>
+      <c r="C76" s="93" t="s">
+        <v>13</v>
+      </c>
+      <c r="D76" s="94"/>
+      <c r="E76" s="94">
+        <v>17</v>
+      </c>
+      <c r="F76" s="94"/>
+      <c r="G76" s="94"/>
+      <c r="H76" s="94"/>
+      <c r="I76" s="94"/>
+    </row>
+    <row r="77" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A77" s="94">
+        <v>32</v>
+      </c>
+      <c r="B77" s="93" t="s">
+        <v>268</v>
+      </c>
+      <c r="C77" s="93" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" s="94"/>
+      <c r="E77" s="94">
+        <v>32</v>
+      </c>
+      <c r="F77" s="94"/>
+      <c r="G77" s="94"/>
+      <c r="H77" s="94"/>
+      <c r="I77" s="94"/>
+    </row>
+    <row r="78" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A78" s="94">
+        <v>33</v>
+      </c>
+      <c r="B78" s="93" t="s">
+        <v>267</v>
+      </c>
+      <c r="C78" s="93" t="s">
+        <v>156</v>
+      </c>
+      <c r="D78" s="94">
+        <v>2</v>
+      </c>
+      <c r="E78" s="94"/>
+      <c r="F78" s="94"/>
+      <c r="G78" s="94"/>
+      <c r="H78" s="94"/>
+      <c r="I78" s="94"/>
+    </row>
+    <row r="79" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A79" s="94">
+        <v>33</v>
+      </c>
+      <c r="B79" s="93" t="s">
+        <v>267</v>
+      </c>
+      <c r="C79" s="93" t="s">
+        <v>156</v>
+      </c>
+      <c r="D79" s="94"/>
+      <c r="E79" s="94">
+        <v>14</v>
+      </c>
+      <c r="F79" s="94"/>
+      <c r="G79" s="94"/>
+      <c r="H79" s="94"/>
+      <c r="I79" s="94"/>
+    </row>
+    <row r="80" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A80" s="94">
+        <v>33</v>
+      </c>
+      <c r="B80" s="93" t="s">
+        <v>275</v>
+      </c>
+      <c r="C80" s="93" t="s">
+        <v>154</v>
+      </c>
+      <c r="D80" s="94"/>
+      <c r="E80" s="94">
+        <v>16</v>
+      </c>
+      <c r="F80" s="94"/>
+      <c r="G80" s="94"/>
+      <c r="H80" s="94"/>
+      <c r="I80" s="94"/>
+    </row>
+    <row r="81" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A81" s="94">
+        <v>33</v>
+      </c>
+      <c r="B81" s="93" t="s">
+        <v>275</v>
+      </c>
+      <c r="C81" s="93" t="s">
+        <v>154</v>
+      </c>
+      <c r="D81" s="94"/>
+      <c r="E81" s="94">
+        <v>29</v>
+      </c>
+      <c r="F81" s="94"/>
+      <c r="G81" s="94"/>
+      <c r="H81" s="94"/>
+      <c r="I81" s="94"/>
+    </row>
+    <row r="82" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A82" s="94">
+        <v>33</v>
+      </c>
+      <c r="B82" s="93" t="s">
+        <v>289</v>
+      </c>
+      <c r="C82" s="93" t="s">
+        <v>156</v>
+      </c>
+      <c r="D82" s="94"/>
+      <c r="E82" s="94">
+        <v>49</v>
+      </c>
+      <c r="F82" s="94"/>
+      <c r="G82" s="94"/>
+      <c r="H82" s="94"/>
+      <c r="I82" s="94"/>
+    </row>
+    <row r="83" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A83" s="94">
+        <v>34</v>
+      </c>
+      <c r="B83" s="93" t="s">
+        <v>290</v>
+      </c>
+      <c r="C83" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="94">
+        <v>30</v>
+      </c>
+      <c r="E83" s="94"/>
+      <c r="F83" s="94"/>
+      <c r="G83" s="94"/>
+      <c r="I83" s="94" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A84" s="94">
+        <v>34</v>
+      </c>
+      <c r="B84" s="93" t="s">
+        <v>291</v>
+      </c>
+      <c r="C84" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84" s="94">
+        <v>48</v>
+      </c>
+      <c r="E84" s="94"/>
+      <c r="F84" s="94"/>
+      <c r="G84" s="94"/>
+      <c r="H84" s="94"/>
+      <c r="I84" s="94"/>
+    </row>
+    <row r="85" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A85" s="94">
+        <v>34</v>
+      </c>
+      <c r="B85" s="93" t="s">
+        <v>292</v>
+      </c>
+      <c r="C85" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" s="94"/>
+      <c r="E85" s="94">
+        <v>11</v>
+      </c>
+      <c r="F85" s="94"/>
+      <c r="G85" s="94"/>
+      <c r="H85" s="94"/>
+      <c r="I85" s="94"/>
+    </row>
+    <row r="86" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A86" s="94">
+        <v>34</v>
+      </c>
+      <c r="B86" s="93" t="s">
+        <v>293</v>
+      </c>
+      <c r="C86" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="94"/>
+      <c r="E86" s="94">
+        <v>22</v>
+      </c>
+      <c r="F86" s="94"/>
+      <c r="G86" s="94"/>
+      <c r="H86" s="94"/>
+      <c r="I86" s="94"/>
+    </row>
+    <row r="87" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A87" s="94">
+        <v>34</v>
+      </c>
+      <c r="B87" s="93" t="s">
+        <v>294</v>
+      </c>
+      <c r="C87" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="D87" s="94"/>
+      <c r="E87" s="94">
+        <v>26</v>
+      </c>
+      <c r="F87" s="94"/>
+      <c r="G87" s="94"/>
+      <c r="I87" s="94" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A88" s="94">
+        <v>35</v>
+      </c>
+      <c r="B88" s="93" t="s">
+        <v>295</v>
+      </c>
+      <c r="C88" s="93" t="s">
+        <v>161</v>
+      </c>
+      <c r="D88" s="94">
+        <v>11</v>
+      </c>
+      <c r="E88" s="94"/>
+      <c r="F88" s="94"/>
+      <c r="G88" s="94"/>
+      <c r="H88" s="94"/>
+      <c r="I88" s="94"/>
+    </row>
+    <row r="89" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A89" s="94">
+        <v>35</v>
+      </c>
+      <c r="B89" s="93" t="s">
+        <v>272</v>
+      </c>
+      <c r="C89" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="D89" s="94"/>
+      <c r="E89" s="94">
+        <v>21</v>
+      </c>
+      <c r="F89" s="94"/>
+      <c r="G89" s="94"/>
+      <c r="H89" s="94"/>
+      <c r="I89" s="94"/>
+    </row>
+    <row r="90" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A90" s="94">
+        <v>35</v>
+      </c>
+      <c r="B90" s="93" t="s">
+        <v>296</v>
+      </c>
+      <c r="C90" s="93" t="s">
+        <v>161</v>
+      </c>
+      <c r="D90" s="94"/>
+      <c r="E90" s="94">
+        <v>23</v>
+      </c>
+      <c r="F90" s="94"/>
+      <c r="G90" s="94"/>
+      <c r="H90" s="94"/>
+      <c r="I90" s="94"/>
+    </row>
+    <row r="91" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A91" s="94">
+        <v>35</v>
+      </c>
+      <c r="B91" s="93" t="s">
+        <v>297</v>
+      </c>
+      <c r="C91" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="D91" s="94"/>
+      <c r="E91" s="94">
+        <v>39</v>
+      </c>
+      <c r="F91" s="94"/>
+      <c r="G91" s="94"/>
+      <c r="H91" s="94"/>
+      <c r="I91" s="94"/>
+    </row>
+    <row r="92" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A92" s="94">
+        <v>36</v>
+      </c>
+      <c r="B92" s="93" t="s">
+        <v>251</v>
+      </c>
+      <c r="C92" s="93" t="s">
+        <v>12</v>
+      </c>
+      <c r="D92" s="94">
+        <v>31</v>
+      </c>
+      <c r="E92" s="94"/>
+      <c r="F92" s="94"/>
+      <c r="G92" s="94"/>
+      <c r="H92" s="94" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A93" s="94">
+        <v>36</v>
+      </c>
+      <c r="B93" s="93" t="s">
+        <v>298</v>
+      </c>
+      <c r="C93" s="93" t="s">
+        <v>11</v>
+      </c>
+      <c r="D93" s="94">
+        <v>47</v>
+      </c>
+      <c r="E93" s="94"/>
+      <c r="F93" s="94"/>
+      <c r="G93" s="94"/>
+      <c r="H93" s="94"/>
+      <c r="I93" s="94"/>
+    </row>
+    <row r="94" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A94" s="94">
+        <v>36</v>
+      </c>
+      <c r="B94" s="93" t="s">
+        <v>298</v>
+      </c>
+      <c r="C94" s="93" t="s">
+        <v>11</v>
+      </c>
+      <c r="D94" s="94"/>
+      <c r="E94" s="94">
+        <v>2</v>
+      </c>
+      <c r="F94" s="94"/>
+      <c r="G94" s="94"/>
+      <c r="H94" s="94" t="s">
+        <v>230</v>
+      </c>
+      <c r="I94" s="94"/>
+    </row>
+    <row r="95" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A95" s="94">
+        <v>36</v>
+      </c>
+      <c r="B95" s="93" t="s">
+        <v>251</v>
+      </c>
+      <c r="C95" s="93" t="s">
+        <v>12</v>
+      </c>
+      <c r="D95" s="94"/>
+      <c r="E95" s="94">
+        <v>15</v>
+      </c>
+      <c r="F95" s="94"/>
+      <c r="G95" s="94"/>
+      <c r="H95" s="94" t="s">
+        <v>230</v>
+      </c>
+      <c r="I95" s="94"/>
+    </row>
+    <row r="96" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A96" s="94">
+        <v>37</v>
+      </c>
+      <c r="B96" s="93" t="s">
+        <v>299</v>
+      </c>
+      <c r="C96" s="93" t="s">
+        <v>198</v>
+      </c>
+      <c r="D96" s="94">
+        <v>27</v>
+      </c>
+      <c r="E96" s="94"/>
+      <c r="F96" s="94"/>
+      <c r="G96" s="94"/>
+      <c r="H96" s="94"/>
+      <c r="I96" s="94"/>
+    </row>
+    <row r="97" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A97" s="94">
+        <v>37</v>
+      </c>
+      <c r="B97" s="93" t="s">
+        <v>285</v>
+      </c>
+      <c r="C97" s="93" t="s">
+        <v>198</v>
+      </c>
+      <c r="D97" s="94"/>
+      <c r="E97" s="94">
+        <v>3</v>
+      </c>
+      <c r="F97" s="94"/>
+      <c r="G97" s="94"/>
+      <c r="H97" s="94"/>
+      <c r="I97" s="94"/>
+    </row>
+    <row r="98" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A98" s="94">
+        <v>37</v>
+      </c>
+      <c r="B98" s="93" t="s">
+        <v>299</v>
+      </c>
+      <c r="C98" s="93" t="s">
+        <v>198</v>
+      </c>
+      <c r="D98" s="94"/>
+      <c r="E98" s="94">
+        <v>43</v>
+      </c>
+      <c r="F98" s="94"/>
+      <c r="G98" s="94"/>
+      <c r="H98" s="94"/>
+      <c r="I98" s="94"/>
+    </row>
+    <row r="99" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A99" s="94">
+        <v>37</v>
+      </c>
+      <c r="B99" s="93" t="s">
+        <v>300</v>
+      </c>
+      <c r="C99" s="93" t="s">
+        <v>198</v>
+      </c>
+      <c r="D99" s="94"/>
+      <c r="E99" s="94">
+        <v>49</v>
+      </c>
+      <c r="F99" s="94"/>
+      <c r="G99" s="94"/>
+      <c r="H99" s="94"/>
+      <c r="I99" s="94"/>
+    </row>
+    <row r="100" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A100" s="94">
+        <v>38</v>
+      </c>
+      <c r="B100" s="93" t="s">
+        <v>301</v>
+      </c>
+      <c r="C100" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D100" s="94"/>
+      <c r="E100" s="94"/>
+      <c r="F100" s="94">
+        <v>5</v>
+      </c>
+      <c r="G100" s="94"/>
+      <c r="H100" s="94"/>
+      <c r="I100" s="94"/>
+    </row>
+    <row r="101" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A101" s="94">
+        <v>38</v>
+      </c>
+      <c r="B101" s="93" t="s">
+        <v>276</v>
+      </c>
+      <c r="C101" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" s="94"/>
+      <c r="E101" s="94"/>
+      <c r="F101" s="94">
+        <v>15</v>
+      </c>
+      <c r="G101" s="94"/>
+      <c r="H101" s="94"/>
+      <c r="I101" s="94"/>
+    </row>
+    <row r="102" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A102" s="94">
+        <v>38</v>
+      </c>
+      <c r="B102" s="93" t="s">
+        <v>302</v>
+      </c>
+      <c r="C102" s="93" t="s">
+        <v>153</v>
+      </c>
+      <c r="D102" s="94"/>
+      <c r="E102" s="94"/>
+      <c r="F102" s="94"/>
+      <c r="G102" s="94">
+        <v>9</v>
+      </c>
+      <c r="H102" s="94"/>
+      <c r="I102" s="94"/>
+    </row>
+    <row r="103" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A103" s="94">
+        <v>39</v>
+      </c>
+      <c r="B103" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="C103" s="93" t="s">
+        <v>157</v>
+      </c>
+      <c r="D103" s="94"/>
+      <c r="E103" s="94">
+        <v>23</v>
+      </c>
+      <c r="F103" s="94"/>
+      <c r="G103" s="94"/>
+      <c r="H103" s="94"/>
+      <c r="I103" s="94"/>
+    </row>
+    <row r="104" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A104" s="94">
+        <v>39</v>
+      </c>
+      <c r="B104" s="93" t="s">
+        <v>246</v>
+      </c>
+      <c r="C104" s="93" t="s">
+        <v>157</v>
+      </c>
+      <c r="D104" s="94"/>
+      <c r="E104" s="94">
+        <v>35</v>
+      </c>
+      <c r="F104" s="94"/>
+      <c r="G104" s="94"/>
+      <c r="H104" s="94"/>
+      <c r="I104" s="94"/>
+    </row>
+    <row r="105" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A105" s="94">
+        <v>40</v>
+      </c>
+      <c r="B105" s="93" t="s">
+        <v>304</v>
+      </c>
+      <c r="C105" s="93" t="s">
+        <v>90</v>
+      </c>
+      <c r="D105" s="94">
+        <v>42</v>
+      </c>
+      <c r="E105" s="94"/>
+      <c r="F105" s="94"/>
+      <c r="G105" s="94"/>
+      <c r="H105" s="94"/>
+      <c r="I105" s="94"/>
+    </row>
+    <row r="106" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A106" s="94">
+        <v>41</v>
+      </c>
+      <c r="B106" s="93" t="s">
+        <v>305</v>
+      </c>
+      <c r="C106" s="93" t="s">
+        <v>13</v>
+      </c>
+      <c r="D106" s="94">
+        <v>20</v>
+      </c>
+      <c r="E106" s="94"/>
+      <c r="F106" s="94"/>
+      <c r="G106" s="94"/>
+      <c r="I106" s="94" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A107" s="94">
+        <v>41</v>
+      </c>
+      <c r="B107" s="93" t="s">
+        <v>292</v>
+      </c>
+      <c r="C107" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107" s="94">
+        <v>38</v>
+      </c>
+      <c r="E107" s="94"/>
+      <c r="F107" s="94"/>
+      <c r="G107" s="94"/>
+      <c r="H107" s="94"/>
+      <c r="I107" s="94"/>
+    </row>
+    <row r="108" spans="1:9" s="95" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A108" s="94">
+        <v>41</v>
+      </c>
+      <c r="B108" s="93" t="s">
+        <v>306</v>
+      </c>
+      <c r="C108" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="D108" s="94"/>
+      <c r="E108" s="94">
+        <v>12</v>
+      </c>
+      <c r="F108" s="94"/>
+      <c r="G108" s="94"/>
+      <c r="H108" s="94"/>
+      <c r="I108" s="94"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A109" s="94">
+        <v>41</v>
+      </c>
+      <c r="B109" s="93" t="s">
+        <v>293</v>
+      </c>
+      <c r="C109" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" s="94">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A110" s="94">
+        <v>41</v>
+      </c>
+      <c r="B110" s="93" t="s">
+        <v>309</v>
+      </c>
+      <c r="C110" s="93" t="s">
+        <v>13</v>
+      </c>
+      <c r="E110" s="94">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" s="94">
+        <v>41</v>
+      </c>
+      <c r="B111" s="93" t="s">
+        <v>310</v>
+      </c>
+      <c r="C111" s="93" t="s">
+        <v>13</v>
+      </c>
+      <c r="E111" s="94">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A112" s="94">
+        <v>41</v>
+      </c>
+      <c r="B112" s="93" t="s">
+        <v>307</v>
+      </c>
+      <c r="C112" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="E112" s="94"/>
+      <c r="F112" s="94">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A113" s="94">
+        <v>41</v>
+      </c>
+      <c r="B113" s="93" t="s">
+        <v>308</v>
+      </c>
+      <c r="C113" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="F113" s="94">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" s="94">
+        <v>42</v>
+      </c>
+      <c r="B114" s="93" t="s">
+        <v>277</v>
+      </c>
+      <c r="C114" s="93" t="s">
+        <v>78</v>
+      </c>
+      <c r="D114" s="94">
+        <v>15</v>
+      </c>
+      <c r="E114" s="94"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" s="94">
+        <v>42</v>
+      </c>
+      <c r="B115" s="93" t="s">
+        <v>298</v>
+      </c>
+      <c r="C115" s="93" t="s">
+        <v>11</v>
+      </c>
+      <c r="D115" s="94"/>
+      <c r="E115" s="94">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A116" s="94">
+        <v>42</v>
+      </c>
+      <c r="B116" s="93" t="s">
+        <v>298</v>
+      </c>
+      <c r="C116" s="93" t="s">
+        <v>11</v>
+      </c>
+      <c r="D116" s="94"/>
+      <c r="E116" s="94">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A117" s="94">
+        <v>42</v>
+      </c>
+      <c r="B117" s="93" t="s">
+        <v>311</v>
+      </c>
+      <c r="C117" s="93" t="s">
+        <v>11</v>
+      </c>
+      <c r="D117" s="94"/>
+      <c r="E117" s="94">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118" s="94">
+        <v>42</v>
+      </c>
+      <c r="B118" s="93" t="s">
+        <v>277</v>
+      </c>
+      <c r="C118" s="93" t="s">
+        <v>78</v>
+      </c>
+      <c r="D118" s="94"/>
+      <c r="E118" s="94">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A119" s="94">
+        <v>42</v>
+      </c>
+      <c r="B119" s="93" t="s">
+        <v>312</v>
+      </c>
+      <c r="C119" s="93" t="s">
+        <v>78</v>
+      </c>
+      <c r="D119" s="94"/>
+      <c r="E119" s="94">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A120" s="94">
+        <v>43</v>
+      </c>
+      <c r="B120" s="93" t="s">
+        <v>236</v>
+      </c>
+      <c r="C120" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="D120" s="94"/>
+      <c r="E120" s="94">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A121" s="94">
+        <v>43</v>
+      </c>
+      <c r="B121" s="93" t="s">
+        <v>313</v>
+      </c>
+      <c r="C121" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="D121" s="94"/>
+      <c r="E121" s="94">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A122" s="94">
+        <v>44</v>
+      </c>
+      <c r="B122" s="93" t="s">
+        <v>314</v>
+      </c>
+      <c r="C122" s="93" t="s">
+        <v>159</v>
+      </c>
+      <c r="D122" s="94">
+        <v>27</v>
+      </c>
+      <c r="E122" s="94"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A123" s="94">
+        <v>44</v>
+      </c>
+      <c r="B123" s="93" t="s">
+        <v>267</v>
+      </c>
+      <c r="C123" s="93" t="s">
+        <v>156</v>
+      </c>
+      <c r="D123" s="94">
+        <v>43</v>
+      </c>
+      <c r="E123" s="94"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A124" s="94">
+        <v>44</v>
+      </c>
+      <c r="B124" s="93" t="s">
+        <v>284</v>
+      </c>
+      <c r="C124" s="93" t="s">
+        <v>159</v>
+      </c>
+      <c r="D124" s="94"/>
+      <c r="E124" s="94"/>
+      <c r="G124" s="94">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A125" s="94">
+        <v>45</v>
+      </c>
+      <c r="B125" s="93" t="s">
+        <v>315</v>
+      </c>
+      <c r="C125" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="D125" s="94">
+        <v>8</v>
+      </c>
+      <c r="E125" s="94"/>
+      <c r="I125" s="94" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A126" s="94">
+        <v>45</v>
+      </c>
+      <c r="B126" s="93" t="s">
+        <v>278</v>
+      </c>
+      <c r="C126" s="93" t="s">
+        <v>78</v>
+      </c>
+      <c r="D126" s="94"/>
+      <c r="E126" s="94">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A127" s="94">
+        <v>46</v>
+      </c>
+      <c r="B127" s="93" t="s">
+        <v>316</v>
+      </c>
+      <c r="C127" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D127" s="94">
+        <v>31</v>
+      </c>
+      <c r="E127" s="94"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A128" s="94">
+        <v>46</v>
+      </c>
+      <c r="B128" s="93" t="s">
+        <v>261</v>
+      </c>
+      <c r="C128" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D128" s="94">
+        <v>44</v>
+      </c>
+      <c r="E128" s="94"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A129" s="94">
+        <v>46</v>
+      </c>
+      <c r="B129" s="93" t="s">
+        <v>234</v>
+      </c>
+      <c r="C129" s="93" t="s">
+        <v>90</v>
+      </c>
+      <c r="D129" s="94">
+        <v>47</v>
+      </c>
+      <c r="E129" s="94"/>
+      <c r="H129" s="94" t="s">
+        <v>230</v>
+      </c>
+      <c r="I129" s="94"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A130" s="94">
+        <v>47</v>
+      </c>
+      <c r="B130" s="93" t="s">
+        <v>317</v>
+      </c>
+      <c r="C130" s="93" t="s">
+        <v>198</v>
+      </c>
+      <c r="D130" s="94">
+        <v>5</v>
+      </c>
+      <c r="E130" s="94"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A131" s="94">
+        <v>47</v>
+      </c>
+      <c r="B131" s="93" t="s">
+        <v>299</v>
+      </c>
+      <c r="C131" s="93" t="s">
+        <v>198</v>
+      </c>
+      <c r="D131" s="94">
+        <v>42</v>
+      </c>
+      <c r="E131" s="94"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A132" s="94">
+        <v>47</v>
+      </c>
+      <c r="B132" s="93" t="s">
+        <v>246</v>
+      </c>
+      <c r="C132" s="93" t="s">
+        <v>157</v>
+      </c>
+      <c r="D132" s="94"/>
+      <c r="E132" s="94">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A133" s="94">
+        <v>48</v>
+      </c>
+      <c r="B133" s="93" t="s">
+        <v>313</v>
+      </c>
+      <c r="C133" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="D133" s="94">
+        <v>4</v>
+      </c>
+      <c r="E133" s="94"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A134" s="94">
+        <v>48</v>
+      </c>
+      <c r="B134" s="93" t="s">
+        <v>318</v>
+      </c>
+      <c r="C134" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="D134" s="94">
+        <v>46</v>
+      </c>
+      <c r="E134" s="94"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A135" s="94">
+        <v>48</v>
+      </c>
+      <c r="B135" s="93" t="s">
+        <v>313</v>
+      </c>
+      <c r="C135" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="D135" s="94"/>
+      <c r="E135" s="94">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A136" s="94">
+        <v>48</v>
+      </c>
+      <c r="B136" s="93" t="s">
+        <v>319</v>
+      </c>
+      <c r="C136" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="D136" s="94"/>
+      <c r="E136" s="94">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A137" s="94">
+        <v>49</v>
+      </c>
+      <c r="B137" s="93" t="s">
+        <v>301</v>
+      </c>
+      <c r="C137" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D137" s="94"/>
+      <c r="E137" s="94">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A138" s="94">
+        <v>49</v>
+      </c>
+      <c r="B138" s="93" t="s">
+        <v>307</v>
+      </c>
+      <c r="C138" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="E138" s="94">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A139" s="94">
+        <v>50</v>
+      </c>
+      <c r="B139" s="93" t="s">
+        <v>282</v>
+      </c>
+      <c r="C139" s="93" t="s">
+        <v>198</v>
+      </c>
+      <c r="E139" s="94">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A140" s="94">
+        <v>50</v>
+      </c>
+      <c r="B140" s="93" t="s">
+        <v>320</v>
+      </c>
+      <c r="C140" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="E140" s="94">
+        <v>39</v>
+      </c>
+      <c r="H140" s="94"/>
+      <c r="I140" s="94" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A141" s="94">
+        <v>50</v>
+      </c>
+      <c r="B141" s="93" t="s">
+        <v>313</v>
+      </c>
+      <c r="C141" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="E141" s="94"/>
+      <c r="F141" s="75">
+        <v>14</v>
+      </c>
+      <c r="H141" s="75" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A142" s="94">
+        <v>51</v>
+      </c>
+      <c r="B142" s="93" t="s">
+        <v>321</v>
+      </c>
+      <c r="C142" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="D142" s="75">
+        <v>2</v>
+      </c>
+      <c r="E142" s="94"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A143" s="94">
+        <v>51</v>
+      </c>
+      <c r="B143" s="93" t="s">
+        <v>322</v>
+      </c>
+      <c r="C143" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="E143" s="94">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A144" s="94"/>
+      <c r="B144" s="93"/>
+      <c r="C144" s="93"/>
+      <c r="E144" s="94"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" s="94"/>
+      <c r="B145" s="93"/>
+      <c r="C145" s="93"/>
+      <c r="E145" s="94"/>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" s="94"/>
+      <c r="B146" s="93"/>
+      <c r="C146" s="93"/>
+      <c r="E146" s="94"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I53" xr:uid="{00000000-0001-0000-0700-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I53">
-    <sortCondition ref="B2:B53"/>
+  <autoFilter ref="A1:I38" xr:uid="{00000000-0001-0000-0700-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I35">
+    <sortCondition ref="B2:B35"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>